<commit_message>
Correct sample update TI volume/delta_volume
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Sample_update_vtest.xlsx
+++ b/backend/fms_core/tests/valid_templates/Sample_update_vtest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmineleblond-chartrand/c3g/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A93669-EE75-DE44-AFDE-FC8E94E29882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802063DE-1F11-A44F-8FB3-BC251D05791C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30980" yWindow="4660" windowWidth="24300" windowHeight="14080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="SampleUpdate" sheetId="1" r:id="rId1"/>
     <sheet name="Index" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -1694,7 +1694,7 @@
   <dimension ref="A1:H391"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1747,9 +1747,7 @@
       <c r="C8" s="4">
         <v>90</v>
       </c>
-      <c r="D8" s="4">
-        <v>9</v>
-      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="4">
         <v>20</v>
       </c>

</xml_diff>